<commit_message>
hieu commit ip changelog
</commit_message>
<xml_diff>
--- a/New_202306/doc/IP_Changelog_CleanIP.xlsx
+++ b/New_202306/doc/IP_Changelog_CleanIP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nthieu\Documents\research\New_202306\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06139BCF-7D63-41D5-A1F4-B0D26458DFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4CE2DB-F059-4272-A970-F90957C6169C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4069EB18-67D6-47EC-BC30-6279B71A6D04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{4069EB18-67D6-47EC-BC30-6279B71A6D04}"/>
   </bookViews>
   <sheets>
     <sheet name="Need_Update" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="119">
   <si>
     <t>Project_Key</t>
   </si>
@@ -346,6 +346,54 @@
   </si>
   <si>
     <t>Gaw NP Industrial</t>
+  </si>
+  <si>
+    <t>Bw Industrial</t>
+  </si>
+  <si>
+    <t>Ktg Industrial</t>
+  </si>
+  <si>
+    <t>Kinh Bac City Development Holding Corporation.</t>
+  </si>
+  <si>
+    <t>Capella Land Jsc</t>
+  </si>
+  <si>
+    <t>KCN Vietnam</t>
+  </si>
+  <si>
+    <t>Kinh Bac City Development Holding Corporation</t>
+  </si>
+  <si>
+    <t>Konoike Vinatrans Logistics Co.,Ltd</t>
+  </si>
+  <si>
+    <t>Le Minh Xuan Ip Jsc</t>
+  </si>
+  <si>
+    <t>Logisvalley Co., Ltd.</t>
+  </si>
+  <si>
+    <t>Npl Logistic Corporation</t>
+  </si>
+  <si>
+    <t>SLP</t>
+  </si>
+  <si>
+    <t>Sojitz</t>
+  </si>
+  <si>
+    <t>Son Ha International Jsc</t>
+  </si>
+  <si>
+    <t>Sonadezi</t>
+  </si>
+  <si>
+    <t>Tin Nghia</t>
+  </si>
+  <si>
+    <t>Tizco</t>
   </si>
 </sst>
 </file>
@@ -734,30 +782,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975D32F1-2779-4398-9D77-FBD428ED1328}">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="9" width="5.140625" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="12" max="17" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -827,33 +862,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5682058B-091E-4FCC-A17B-606BC86F242E}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1658,6 +1673,832 @@
       </c>
       <c r="R36" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5056</v>
+      </c>
+      <c r="J37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
+        <v>101</v>
+      </c>
+      <c r="R37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3700</v>
+      </c>
+      <c r="J38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" t="s">
+        <v>101</v>
+      </c>
+      <c r="R38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3728</v>
+      </c>
+      <c r="J39" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" t="s">
+        <v>101</v>
+      </c>
+      <c r="R39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3761</v>
+      </c>
+      <c r="J40" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" t="s">
+        <v>101</v>
+      </c>
+      <c r="R40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3762</v>
+      </c>
+      <c r="J41" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" t="s">
+        <v>101</v>
+      </c>
+      <c r="R41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3763</v>
+      </c>
+      <c r="J42" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" t="s">
+        <v>101</v>
+      </c>
+      <c r="R42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3764</v>
+      </c>
+      <c r="J43" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" t="s">
+        <v>101</v>
+      </c>
+      <c r="R43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3796</v>
+      </c>
+      <c r="J44" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" t="s">
+        <v>101</v>
+      </c>
+      <c r="R44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3802</v>
+      </c>
+      <c r="J45" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" t="s">
+        <v>101</v>
+      </c>
+      <c r="R45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3804</v>
+      </c>
+      <c r="J46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K46" t="s">
+        <v>101</v>
+      </c>
+      <c r="R46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3822</v>
+      </c>
+      <c r="J47" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" t="s">
+        <v>101</v>
+      </c>
+      <c r="R47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3873</v>
+      </c>
+      <c r="J48" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" t="s">
+        <v>101</v>
+      </c>
+      <c r="R48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3895</v>
+      </c>
+      <c r="J49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" t="s">
+        <v>101</v>
+      </c>
+      <c r="R49" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3949</v>
+      </c>
+      <c r="J50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" t="s">
+        <v>101</v>
+      </c>
+      <c r="R50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3978</v>
+      </c>
+      <c r="J51" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" t="s">
+        <v>101</v>
+      </c>
+      <c r="R51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3979</v>
+      </c>
+      <c r="J52" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" t="s">
+        <v>101</v>
+      </c>
+      <c r="R52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4161</v>
+      </c>
+      <c r="J53" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" t="s">
+        <v>101</v>
+      </c>
+      <c r="R53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>4166</v>
+      </c>
+      <c r="J54" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" t="s">
+        <v>101</v>
+      </c>
+      <c r="R54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>4200</v>
+      </c>
+      <c r="J55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" t="s">
+        <v>101</v>
+      </c>
+      <c r="R55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4491</v>
+      </c>
+      <c r="J56" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s">
+        <v>101</v>
+      </c>
+      <c r="R56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4512</v>
+      </c>
+      <c r="J57" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" t="s">
+        <v>101</v>
+      </c>
+      <c r="R57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>4646</v>
+      </c>
+      <c r="J58" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" t="s">
+        <v>101</v>
+      </c>
+      <c r="R58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4647</v>
+      </c>
+      <c r="J59" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" t="s">
+        <v>101</v>
+      </c>
+      <c r="R59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>4648</v>
+      </c>
+      <c r="J60" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" t="s">
+        <v>101</v>
+      </c>
+      <c r="R60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>4649</v>
+      </c>
+      <c r="J61" t="s">
+        <v>20</v>
+      </c>
+      <c r="K61" t="s">
+        <v>101</v>
+      </c>
+      <c r="R61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>4650</v>
+      </c>
+      <c r="J62" t="s">
+        <v>20</v>
+      </c>
+      <c r="K62" t="s">
+        <v>101</v>
+      </c>
+      <c r="R62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>4669</v>
+      </c>
+      <c r="J63" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" t="s">
+        <v>101</v>
+      </c>
+      <c r="R63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>4670</v>
+      </c>
+      <c r="J64" t="s">
+        <v>20</v>
+      </c>
+      <c r="K64" t="s">
+        <v>101</v>
+      </c>
+      <c r="R64" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>4711</v>
+      </c>
+      <c r="J65" t="s">
+        <v>20</v>
+      </c>
+      <c r="K65" t="s">
+        <v>101</v>
+      </c>
+      <c r="R65" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>4717</v>
+      </c>
+      <c r="J66" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s">
+        <v>101</v>
+      </c>
+      <c r="R66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>4752</v>
+      </c>
+      <c r="J67" t="s">
+        <v>20</v>
+      </c>
+      <c r="K67" t="s">
+        <v>101</v>
+      </c>
+      <c r="R67" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>4796</v>
+      </c>
+      <c r="J68" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" t="s">
+        <v>101</v>
+      </c>
+      <c r="R68" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>4797</v>
+      </c>
+      <c r="J69" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" t="s">
+        <v>101</v>
+      </c>
+      <c r="R69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>5162</v>
+      </c>
+      <c r="J70" t="s">
+        <v>20</v>
+      </c>
+      <c r="K70" t="s">
+        <v>101</v>
+      </c>
+      <c r="R70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5283</v>
+      </c>
+      <c r="J71" t="s">
+        <v>20</v>
+      </c>
+      <c r="K71" t="s">
+        <v>101</v>
+      </c>
+      <c r="R71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>4799</v>
+      </c>
+      <c r="J72" t="s">
+        <v>20</v>
+      </c>
+      <c r="K72" t="s">
+        <v>101</v>
+      </c>
+      <c r="R72" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>5280</v>
+      </c>
+      <c r="J73" t="s">
+        <v>20</v>
+      </c>
+      <c r="K73" t="s">
+        <v>101</v>
+      </c>
+      <c r="R73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>5281</v>
+      </c>
+      <c r="J74" t="s">
+        <v>20</v>
+      </c>
+      <c r="K74" t="s">
+        <v>101</v>
+      </c>
+      <c r="R74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>4706</v>
+      </c>
+      <c r="J75" t="s">
+        <v>20</v>
+      </c>
+      <c r="K75" t="s">
+        <v>101</v>
+      </c>
+      <c r="R75" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>5149</v>
+      </c>
+      <c r="J76" t="s">
+        <v>20</v>
+      </c>
+      <c r="K76" t="s">
+        <v>101</v>
+      </c>
+      <c r="R76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>5280</v>
+      </c>
+      <c r="J77" t="s">
+        <v>20</v>
+      </c>
+      <c r="K77" t="s">
+        <v>101</v>
+      </c>
+      <c r="R77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>5281</v>
+      </c>
+      <c r="J78" t="s">
+        <v>20</v>
+      </c>
+      <c r="K78" t="s">
+        <v>101</v>
+      </c>
+      <c r="R78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>4156</v>
+      </c>
+      <c r="J79" t="s">
+        <v>20</v>
+      </c>
+      <c r="K79" t="s">
+        <v>101</v>
+      </c>
+      <c r="R79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>4181</v>
+      </c>
+      <c r="J80" t="s">
+        <v>20</v>
+      </c>
+      <c r="K80" t="s">
+        <v>101</v>
+      </c>
+      <c r="R80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>4641</v>
+      </c>
+      <c r="J81" t="s">
+        <v>20</v>
+      </c>
+      <c r="K81" t="s">
+        <v>101</v>
+      </c>
+      <c r="R81" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2742</v>
+      </c>
+      <c r="J82" t="s">
+        <v>20</v>
+      </c>
+      <c r="K82" t="s">
+        <v>101</v>
+      </c>
+      <c r="R82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>5294</v>
+      </c>
+      <c r="J83" t="s">
+        <v>20</v>
+      </c>
+      <c r="K83" t="s">
+        <v>101</v>
+      </c>
+      <c r="R83" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>3928</v>
+      </c>
+      <c r="J84" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" t="s">
+        <v>101</v>
+      </c>
+      <c r="R84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>4163</v>
+      </c>
+      <c r="J85" t="s">
+        <v>20</v>
+      </c>
+      <c r="K85" t="s">
+        <v>101</v>
+      </c>
+      <c r="R85" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>5144</v>
+      </c>
+      <c r="J86" t="s">
+        <v>20</v>
+      </c>
+      <c r="K86" t="s">
+        <v>101</v>
+      </c>
+      <c r="R86" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>3051</v>
+      </c>
+      <c r="J87" t="s">
+        <v>20</v>
+      </c>
+      <c r="K87" t="s">
+        <v>101</v>
+      </c>
+      <c r="R87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>3773</v>
+      </c>
+      <c r="J88" t="s">
+        <v>20</v>
+      </c>
+      <c r="K88" t="s">
+        <v>101</v>
+      </c>
+      <c r="R88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3800</v>
+      </c>
+      <c r="J89" t="s">
+        <v>20</v>
+      </c>
+      <c r="K89" t="s">
+        <v>101</v>
+      </c>
+      <c r="R89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>3803</v>
+      </c>
+      <c r="J90" t="s">
+        <v>20</v>
+      </c>
+      <c r="K90" t="s">
+        <v>101</v>
+      </c>
+      <c r="R90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>4281</v>
+      </c>
+      <c r="J91" t="s">
+        <v>20</v>
+      </c>
+      <c r="K91" t="s">
+        <v>101</v>
+      </c>
+      <c r="R91" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>3734</v>
+      </c>
+      <c r="J92" t="s">
+        <v>20</v>
+      </c>
+      <c r="K92" t="s">
+        <v>101</v>
+      </c>
+      <c r="R92" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>3745</v>
+      </c>
+      <c r="J93" t="s">
+        <v>20</v>
+      </c>
+      <c r="K93" t="s">
+        <v>101</v>
+      </c>
+      <c r="R93" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3750</v>
+      </c>
+      <c r="J94" t="s">
+        <v>20</v>
+      </c>
+      <c r="K94" t="s">
+        <v>101</v>
+      </c>
+      <c r="R94" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2863</v>
+      </c>
+      <c r="J95" t="s">
+        <v>20</v>
+      </c>
+      <c r="K95" t="s">
+        <v>101</v>
+      </c>
+      <c r="R95" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1917,6 +2758,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="83ed40fe-a0b7-48db-98c8-b545194bd4ce">
@@ -1925,15 +2775,6 @@
     <TaxCatchAll xmlns="b3546b15-478d-4407-9e3d-dd057d7f6994" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1957,6 +2798,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0458A1-5C95-4377-84EE-AC390C92EAFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F45F6EB9-5718-4E3A-9EED-7CCC2079CE77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1965,12 +2814,4 @@
     <ds:schemaRef ds:uri="b3546b15-478d-4407-9e3d-dd057d7f6994"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0458A1-5C95-4377-84EE-AC390C92EAFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>